<commit_message>
Update transcriptomics metadata template: limit the range of values.
</commit_message>
<xml_diff>
--- a/public/metadata-templates/transcriptomics-metadata-template.xlsx
+++ b/public/metadata-templates/transcriptomics-metadata-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/choppy/Documents/Code/ChineseQuartet/quartet-studio/public/metadata-templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB16CE22-9498-2D42-A65C-C1CD4EBA6F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE14781E-AF34-6544-966E-81B48C362BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="520" windowWidth="26880" windowHeight="16280" xr2:uid="{A58EA485-3F1D-4B3F-B94B-7C41644033AE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="16300" activeTab="2" xr2:uid="{A58EA485-3F1D-4B3F-B94B-7C41644033AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Please Read First!" sheetId="5" r:id="rId1"/>
@@ -1230,7 +1230,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64F19F2F-4205-8046-8351-0FE58B3231A2}">
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:G3"/>
     </sheetView>
   </sheetViews>
@@ -2447,8 +2447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66EA9666-A0F9-934D-B4B5-980441048860}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2537,39 +2537,39 @@
       <c r="J5" s="54"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="UOkA7VjTJzNvP6fzWVHGxAS/QSvE1mrvZvr7b0pSvvlYHZE3F4OoB1KokRekG5GFH/d+diadZIJey0rWksU2jw==" saltValue="j7Trzj9OjEyFVKNQVHxwBA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="YJ2/jV20txkuz8QDu4hv2631AOgjdkE7AkLyTOUP0FOwQw/cQXuSIzgBOTBm8uuVprgPObKqKBO7PD8L4iJqSA==" saltValue="tas0WIJSaja3LmbwR3nidg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <dataValidations count="9">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="RIN" prompt="e.g 10.0" sqref="B2:B1048576" xr:uid="{394E9430-2ADC-0A41-8DB5-FC4B763F016E}">
-      <formula1>0</formula1>
-      <formula2>100</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="RNA conc. (ng/uL)" prompt="e.g 500" sqref="C2:C1048576" xr:uid="{ED79C33F-54D1-F84F-9FFF-E8ACC2A615C1}">
-      <formula1>0</formula1>
-      <formula2>10000</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="RNA volume (uL)" prompt="e.g. 10" sqref="D2:D1048576" xr:uid="{E91F1BF2-4A6C-9A46-BE59-522B88A2B476}">
-      <formula1>0</formula1>
-      <formula2>10000</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="cDNA fragments (bp)" prompt="e.g. 350" sqref="E2:E1048576" xr:uid="{B1F12F3D-E149-FA4E-B2FE-F8B5F8C46E9A}">
-      <formula1>0</formula1>
-      <formula2>10000</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="cDNA conc. (ng/uL)" prompt="e.g. 20" sqref="F2:F1048576" xr:uid="{1670F253-09E1-5344-9FFE-612969BABC9D}">
-      <formula1>0</formula1>
-      <formula2>10000</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="cDNA volume (uL)" prompt="e.g. 22" sqref="G2:G1048576" xr:uid="{35EF15A9-03D7-204C-AFEE-12B8F1FC63B4}">
-      <formula1>0</formula1>
-      <formula2>10000</formula2>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Between 1 and 10." promptTitle="RIN" prompt="e.g 10.0" sqref="B2:B1048576" xr:uid="{394E9430-2ADC-0A41-8DB5-FC4B763F016E}">
+      <formula1>1</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Between 100 and 1000" promptTitle="RNA conc. (ng/uL)" prompt="e.g 500" sqref="C2:C1048576" xr:uid="{ED79C33F-54D1-F84F-9FFF-E8ACC2A615C1}">
+      <formula1>100</formula1>
+      <formula2>1000</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Between 10 and 50." promptTitle="RNA volume (uL)" prompt="e.g. 10" sqref="D2:D1048576" xr:uid="{E91F1BF2-4A6C-9A46-BE59-522B88A2B476}">
+      <formula1>10</formula1>
+      <formula2>50</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Between 100 and 1000" promptTitle="cDNA fragments (bp)" prompt="e.g. 350" sqref="E2:E1048576" xr:uid="{B1F12F3D-E149-FA4E-B2FE-F8B5F8C46E9A}">
+      <formula1>100</formula1>
+      <formula2>1000</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Between 0.1 and 200" promptTitle="cDNA conc. (ng/uL)" prompt="e.g. 20" sqref="F2:F1048576" xr:uid="{1670F253-09E1-5344-9FFE-612969BABC9D}">
+      <formula1>0.1</formula1>
+      <formula2>200</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Between 1 and 50" promptTitle="cDNA volume (uL)" prompt="e.g. 22" sqref="G2:G1048576" xr:uid="{35EF15A9-03D7-204C-AFEE-12B8F1FC63B4}">
+      <formula1>1</formula1>
+      <formula2>50</formula2>
     </dataValidation>
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="cDNA yield (ng)" prompt="e.g. 440" sqref="H2:H1048576" xr:uid="{B0D03BCA-81D0-EF49-A76D-FFAD2AC7AF2B}">
       <formula1>0</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Q30" prompt="e.g. 95" sqref="I2:I1048576" xr:uid="{F2BECAE4-62D8-7C47-B231-8184D82B6FAB}">
-      <formula1>0</formula1>
-      <formula2>1000</formula2>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Between 80 and 100" promptTitle="Q30" prompt="e.g. 95" sqref="I2:I1048576" xr:uid="{F2BECAE4-62D8-7C47-B231-8184D82B6FAB}">
+      <formula1>80</formula1>
+      <formula2>100</formula2>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="total reads (M)" prompt="e.g. 36363" sqref="J2:J1048576" xr:uid="{F20C3780-45C9-BC4D-889E-4CCAFA7B1495}">
       <formula1>0</formula1>

</xml_diff>

<commit_message>
Update transcriptomics metadata template: wrong data type.
</commit_message>
<xml_diff>
--- a/public/metadata-templates/transcriptomics-metadata-template.xlsx
+++ b/public/metadata-templates/transcriptomics-metadata-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/choppy/Documents/Code/ChineseQuartet/quartet-studio/public/metadata-templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE14781E-AF34-6544-966E-81B48C362BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB727DE-56BE-414A-A0A1-0B61D59402E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="16300" activeTab="2" xr2:uid="{A58EA485-3F1D-4B3F-B94B-7C41644033AE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="16300" activeTab="1" xr2:uid="{A58EA485-3F1D-4B3F-B94B-7C41644033AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Please Read First!" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="161">
   <si>
     <t>sample_id</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -505,12 +505,51 @@
 NOTE: This template table may change in the future as the specification is upgraded (Current Version: 20220505)</t>
     </r>
   </si>
+  <si>
+    <t>Vazeme</t>
+  </si>
+  <si>
+    <t>VAHTS mRNA Capture Beads</t>
+  </si>
+  <si>
+    <t>N401</t>
+  </si>
+  <si>
+    <t>VAHTS RNA Clean Beads</t>
+  </si>
+  <si>
+    <t>N412</t>
+  </si>
+  <si>
+    <t>Vazyme</t>
+  </si>
+  <si>
+    <t>VAHTS Universal V8 RNA-seq Library Prep Kit for Illumina</t>
+  </si>
+  <si>
+    <t>NR605</t>
+  </si>
+  <si>
+    <t>VAHTS RNA Multiplex Oligos Set1- Set2 for Illumina</t>
+  </si>
+  <si>
+    <t>N323</t>
+  </si>
+  <si>
+    <t>VAHTS DNA Clean Beads</t>
+  </si>
+  <si>
+    <t>N411</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NovaSeq 6000 S4 Reagent Kit v1.5 (300 cycles) </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -632,6 +671,18 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -829,87 +880,85 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="19" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1231,7 +1280,7 @@
   <dimension ref="A1:G68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:G3"/>
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="34.6640625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1247,48 +1296,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
     </row>
     <row r="2" spans="1:7" s="8" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="42" t="s">
         <v>147</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
     </row>
     <row r="3" spans="1:7" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
     </row>
     <row r="4" spans="1:7" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
     </row>
     <row r="5" spans="1:7" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
@@ -1431,6 +1480,9 @@
       <c r="D12" s="8" t="s">
         <v>36</v>
       </c>
+      <c r="E12" s="8">
+        <v>100</v>
+      </c>
     </row>
     <row r="13" spans="1:7" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
@@ -1462,6 +1514,12 @@
       <c r="C14" s="16" t="s">
         <v>75</v>
       </c>
+      <c r="D14" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="15" spans="1:7" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
@@ -1473,6 +1531,12 @@
       <c r="C15" s="16" t="s">
         <v>75</v>
       </c>
+      <c r="D15" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="16" spans="1:7" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
@@ -1484,6 +1548,12 @@
       <c r="C16" s="16" t="s">
         <v>75</v>
       </c>
+      <c r="D16" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="17" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
@@ -1495,6 +1565,9 @@
       <c r="C17" s="16" t="s">
         <v>75</v>
       </c>
+      <c r="D17" s="17" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
@@ -1506,6 +1579,12 @@
       <c r="C18" s="16" t="s">
         <v>75</v>
       </c>
+      <c r="D18" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="19" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
@@ -1517,6 +1596,12 @@
       <c r="C19" s="16" t="s">
         <v>75</v>
       </c>
+      <c r="D19" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="40" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="20" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
@@ -1528,6 +1613,12 @@
       <c r="C20" s="16" t="s">
         <v>75</v>
       </c>
+      <c r="D20" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="17">
+        <v>85</v>
+      </c>
     </row>
     <row r="21" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
@@ -1539,6 +1630,12 @@
       <c r="C21" s="16" t="s">
         <v>75</v>
       </c>
+      <c r="D21" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="17">
+        <v>5</v>
+      </c>
     </row>
     <row r="22" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
@@ -1550,6 +1647,12 @@
       <c r="C22" s="16" t="s">
         <v>75</v>
       </c>
+      <c r="D22" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="17">
+        <v>20200808</v>
+      </c>
     </row>
     <row r="23" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
@@ -1595,6 +1698,12 @@
       <c r="C25" s="19" t="s">
         <v>97</v>
       </c>
+      <c r="D25" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25" s="40" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="26" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
@@ -1606,6 +1715,12 @@
       <c r="C26" s="19" t="s">
         <v>97</v>
       </c>
+      <c r="D26" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" s="61" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="27" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
@@ -1617,6 +1732,12 @@
       <c r="C27" s="19" t="s">
         <v>97</v>
       </c>
+      <c r="D27" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" s="40" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="28" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
@@ -1628,6 +1749,9 @@
       <c r="C28" s="19" t="s">
         <v>97</v>
       </c>
+      <c r="D28" s="17" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="29" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
@@ -1639,6 +1763,12 @@
       <c r="C29" s="19" t="s">
         <v>97</v>
       </c>
+      <c r="D29" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29" s="40" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="30" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="15" t="s">
@@ -1650,6 +1780,12 @@
       <c r="C30" s="19" t="s">
         <v>97</v>
       </c>
+      <c r="D30" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E30" s="61" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="31" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
@@ -1661,6 +1797,12 @@
       <c r="C31" s="19" t="s">
         <v>97</v>
       </c>
+      <c r="D31" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" s="40" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="32" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="15" t="s">
@@ -1672,6 +1814,12 @@
       <c r="C32" s="19" t="s">
         <v>97</v>
       </c>
+      <c r="D32" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E32" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="15" t="s">
@@ -1683,6 +1831,12 @@
       <c r="C33" s="19" t="s">
         <v>97</v>
       </c>
+      <c r="D33" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E33" s="40" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="34" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="15" t="s">
@@ -1694,6 +1848,12 @@
       <c r="C34" s="19" t="s">
         <v>97</v>
       </c>
+      <c r="D34" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E34" s="61" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="35" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="15" t="s">
@@ -1705,6 +1865,12 @@
       <c r="C35" s="19" t="s">
         <v>97</v>
       </c>
+      <c r="D35" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E35" s="40" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="36" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="15" t="s">
@@ -1716,6 +1882,12 @@
       <c r="C36" s="19" t="s">
         <v>97</v>
       </c>
+      <c r="D36" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E36" s="17">
+        <v>5</v>
+      </c>
     </row>
     <row r="37" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="15" t="s">
@@ -1727,6 +1899,12 @@
       <c r="C37" s="19" t="s">
         <v>97</v>
       </c>
+      <c r="D37" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="E37" s="40" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="38" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="15" t="s">
@@ -1738,6 +1916,12 @@
       <c r="C38" s="19" t="s">
         <v>97</v>
       </c>
+      <c r="D38" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E38" s="40" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="39" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="15" t="s">
@@ -1749,6 +1933,12 @@
       <c r="C39" s="19" t="s">
         <v>97</v>
       </c>
+      <c r="D39" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E39" s="17">
+        <v>13</v>
+      </c>
     </row>
     <row r="40" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="15" t="s">
@@ -1760,6 +1950,12 @@
       <c r="C40" s="19" t="s">
         <v>97</v>
       </c>
+      <c r="D40" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E40" s="17">
+        <v>7.5</v>
+      </c>
     </row>
     <row r="41" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="15" t="s">
@@ -1771,6 +1967,12 @@
       <c r="C41" s="19" t="s">
         <v>97</v>
       </c>
+      <c r="D41" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E41" s="17">
+        <v>15</v>
+      </c>
     </row>
     <row r="42" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="15" t="s">
@@ -1782,6 +1984,12 @@
       <c r="C42" s="19" t="s">
         <v>97</v>
       </c>
+      <c r="D42" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E42" s="17">
+        <v>20200808</v>
+      </c>
     </row>
     <row r="43" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="15" t="s">
@@ -1793,6 +2001,12 @@
       <c r="C43" s="19" t="s">
         <v>97</v>
       </c>
+      <c r="D43" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="44" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="20" t="s">
@@ -1858,6 +2072,12 @@
       <c r="C47" s="21" t="s">
         <v>94</v>
       </c>
+      <c r="D47" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E47" s="61" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="48" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="15" t="s">
@@ -1869,6 +2089,12 @@
       <c r="C48" s="21" t="s">
         <v>94</v>
       </c>
+      <c r="D48" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E48" s="40">
+        <v>20028312</v>
+      </c>
     </row>
     <row r="49" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="15" t="s">
@@ -1908,6 +2134,12 @@
       <c r="C51" s="21" t="s">
         <v>94</v>
       </c>
+      <c r="D51" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E51" s="17">
+        <v>150</v>
+      </c>
     </row>
     <row r="52" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="15" t="s">
@@ -1919,6 +2151,9 @@
       <c r="C52" s="21" t="s">
         <v>94</v>
       </c>
+      <c r="D52" s="17" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="53" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="15" t="s">
@@ -1930,6 +2165,9 @@
       <c r="C53" s="21" t="s">
         <v>94</v>
       </c>
+      <c r="D53" s="17" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="54" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="15" t="s">
@@ -1944,6 +2182,9 @@
       <c r="D54" s="22" t="s">
         <v>36</v>
       </c>
+      <c r="E54" s="17">
+        <v>20200808</v>
+      </c>
     </row>
     <row r="55" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="22"/>
@@ -1954,14 +2195,14 @@
       <c r="C56" s="22"/>
     </row>
     <row r="57" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="60" t="s">
+      <c r="A57" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="B57" s="60"/>
-      <c r="C57" s="60"/>
-      <c r="D57" s="60"/>
-      <c r="E57" s="60"/>
-      <c r="F57" s="60"/>
+      <c r="B57" s="44"/>
+      <c r="C57" s="44"/>
+      <c r="D57" s="44"/>
+      <c r="E57" s="44"/>
+      <c r="F57" s="44"/>
     </row>
     <row r="58" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="9" t="s">
@@ -1994,6 +2235,9 @@
       <c r="D59" s="17" t="s">
         <v>35</v>
       </c>
+      <c r="E59" s="6" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="60" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="23" t="s">
@@ -2150,7 +2394,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="0psQEcEfSGNrW23QQmtmGSz/jjL5o4K9SIBLwz1XNzCNGbkpgZ3tyzRUxkpEzbdZPJqcEXcbCDywJ7GQWL8bGQ==" saltValue="rweyWWM9hDTKROB/nu3L0g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="N0BtLGdWGAo56rAxBtdT0fUM8P0Sab7ZHYtlhuU3zw/NZ1EVMspFQF91bV/sBhX8fvMhzYmdxWikmYqSVc6Mlg==" saltValue="X7C9JnUdgrH+3aaOLEOf1g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="5">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
@@ -2167,21 +2411,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ECE994F-BB82-2E4E-84AB-792F6F7C8F43}">
   <dimension ref="A1:AW1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="AL2" sqref="AL2:AL1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.83203125" defaultRowHeight="26" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="24.83203125" style="40"/>
-    <col min="6" max="6" width="24.83203125" style="41"/>
-    <col min="7" max="14" width="24.83203125" style="42"/>
-    <col min="15" max="16" width="24.83203125" style="43"/>
-    <col min="17" max="18" width="24.83203125" style="42"/>
-    <col min="19" max="38" width="24.83203125" style="44"/>
-    <col min="39" max="47" width="24.83203125" style="45"/>
-    <col min="48" max="49" width="24.83203125" style="46"/>
-    <col min="50" max="16384" width="24.83203125" style="47"/>
+    <col min="1" max="5" width="24.83203125" style="54"/>
+    <col min="6" max="6" width="24.83203125" style="55"/>
+    <col min="7" max="14" width="24.83203125" style="56"/>
+    <col min="15" max="16" width="24.83203125" style="57"/>
+    <col min="17" max="18" width="24.83203125" style="56"/>
+    <col min="19" max="26" width="24.83203125" style="58"/>
+    <col min="27" max="27" width="24.83203125" style="59"/>
+    <col min="28" max="38" width="24.83203125" style="58"/>
+    <col min="39" max="47" width="24.83203125" style="52"/>
+    <col min="48" max="49" width="24.83203125" style="60"/>
+    <col min="50" max="16384" width="24.83203125" style="49"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:49" s="6" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -2334,7 +2580,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Naec8xg6LTAVr1DucbkKnYlv5/gFSMy2vGqJnrzX5dHHBIFrbrq8sjRnGa4Sz6qsPPKebIiaXh6YhDc7iIIBGQ==" saltValue="rgAweEIFeqRfqdtinBe1aQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="dzcmAfGou4weLrVvywGvnQuR58ds7aGJNoG2Slxtp8/KVs+eOWKsJP/3yNsXFmAFlaVNFnKZgJxX7QOp8aVMJA==" saltValue="TS0L2MsAB7gnj79lYkTz/g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="45">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="&lt;lab-name&gt;_Illumina_D5_&lt;sequencing-date&gt;_&lt;no.&gt;_R1/R2.fastq.gz_x000d__x000a__x000d__x000a_e.g FDU_Illumina_D5_20200808_001_R1.fastq.gz" sqref="B2:B1048576" xr:uid="{EE4EBFB8-3AF4-9545-A3BA-CB54EA5CFE04}"/>
@@ -2374,10 +2620,10 @@
       <formula2>21000000</formula2>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Is automation?" prompt="e.g. TRUE" sqref="R2:R1048576" xr:uid="{75FDDACF-6B09-C24D-98C5-AA2BA50E61AE}">
-      <formula1>"TRUE/FALSE"</formula1>
+      <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Is strand specific?" prompt="e.g. TRUE" sqref="S2:S1048576" xr:uid="{56529B1E-7C9A-D842-9445-6B685BFFA2C5}">
-      <formula1>"TRUE/FALSE"</formula1>
+      <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Manufacturer for RNAseq library" prompt="e.g. Vazyme" sqref="T2:T1048576" xr:uid="{E888C1FF-0889-9C4D-B2DD-12539CFFF712}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="RNAseq library prep kit" prompt="VAHTS Universal V8 RNA-seq Library Prep Kit for Illumina" sqref="U2:U1048576" xr:uid="{E86A56E8-0C58-2C46-996E-B73D40E30AC3}"/>
@@ -2415,7 +2661,7 @@
       <formula2>21000000</formula2>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2:AL1048576" xr:uid="{B4EB32C1-D74B-8E49-B11C-C4C5C43ADEBD}">
-      <formula1>"TRUE/FALSE"</formula1>
+      <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Manufacturer for sequencer" prompt="e.g. Illumina" sqref="AM2:AM1048576" xr:uid="{D9C6F851-7E62-1B48-B1A2-9EC369BEA4B9}">
       <formula1>"Illumina,MGI"</formula1>
@@ -2445,19 +2691,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66EA9666-A0F9-934D-B4B5-980441048860}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="47"/>
-    <col min="2" max="4" width="20.6640625" style="45"/>
-    <col min="5" max="8" width="20.6640625" style="55"/>
-    <col min="9" max="10" width="20.6640625" style="56"/>
-    <col min="11" max="16384" width="20.6640625" style="51"/>
+    <col min="1" max="1" width="20.6640625" style="49"/>
+    <col min="2" max="4" width="20.6640625" style="52"/>
+    <col min="5" max="8" width="20.6640625" style="53"/>
+    <col min="9" max="10" width="20.6640625" style="48"/>
+    <col min="11" max="16384" width="20.6640625" style="47"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2493,51 +2739,18 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-    </row>
-    <row r="3" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-    </row>
-    <row r="4" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-    </row>
-    <row r="5" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="54"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="YJ2/jV20txkuz8QDu4hv2631AOgjdkE7AkLyTOUP0FOwQw/cQXuSIzgBOTBm8uuVprgPObKqKBO7PD8L4iJqSA==" saltValue="tas0WIJSaja3LmbwR3nidg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="/c/p3vurwIDKYkaMV70rveWOgGayM+u2lEe9LX1UjTBPjUenRCBWQzVLynBoreHbIMczw3qiCjZ8pJ0vOVVwNg==" saltValue="E8OgBx0mVtKE+UgmG47uCw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <dataValidations count="9">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Between 1 and 10." promptTitle="RIN" prompt="e.g 10.0" sqref="B2:B1048576" xr:uid="{394E9430-2ADC-0A41-8DB5-FC4B763F016E}">
       <formula1>1</formula1>

</xml_diff>

<commit_message>
Update transcriptomics metadata template: fix spelling errors.
</commit_message>
<xml_diff>
--- a/public/metadata-templates/transcriptomics-metadata-template.xlsx
+++ b/public/metadata-templates/transcriptomics-metadata-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/choppy/Documents/Code/ChineseQuartet/quartet-studio/public/metadata-templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB727DE-56BE-414A-A0A1-0B61D59402E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EAE7600-353B-3C4C-9A90-A9AFDE784D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="16300" activeTab="1" xr2:uid="{A58EA485-3F1D-4B3F-B94B-7C41644033AE}"/>
   </bookViews>
@@ -215,9 +215,6 @@
     <t>enrichment_date</t>
   </si>
   <si>
-    <t>is_automation</t>
-  </si>
-  <si>
     <t>is_strand_specific</t>
   </si>
   <si>
@@ -272,9 +269,6 @@
     <t>TRUE/FALSE</t>
   </si>
   <si>
-    <t>library_is_automation</t>
-  </si>
-  <si>
     <t>library_clean_beads</t>
   </si>
   <si>
@@ -377,9 +371,6 @@
     <t>Date for RNA enrichments</t>
   </si>
   <si>
-    <t>Is Automation?</t>
-  </si>
-  <si>
     <t>Is strand-specific?</t>
   </si>
   <si>
@@ -426,9 +417,6 @@
   </si>
   <si>
     <t>Date for RNAseq preparation</t>
-  </si>
-  <si>
-    <t>Is automation?</t>
   </si>
   <si>
     <t>Manufacturer for sequencer</t>
@@ -543,6 +531,18 @@
   </si>
   <si>
     <t xml:space="preserve">NovaSeq 6000 S4 Reagent Kit v1.5 (300 cycles) </t>
+  </si>
+  <si>
+    <t>library_is_automated</t>
+  </si>
+  <si>
+    <t>is_automated</t>
+  </si>
+  <si>
+    <t>Manual/Automated</t>
+  </si>
+  <si>
+    <t>Manual or automated</t>
   </si>
 </sst>
 </file>
@@ -883,21 +883,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -959,6 +944,21 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1280,7 +1280,7 @@
   <dimension ref="A1:G68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="34.6640625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1296,48 +1296,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
     </row>
     <row r="2" spans="1:7" s="8" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
-        <v>147</v>
-      </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
+      <c r="A2" s="58" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
     </row>
     <row r="3" spans="1:7" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
     </row>
     <row r="4" spans="1:7" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="45" t="s">
-        <v>98</v>
-      </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
+      <c r="A4" s="61" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
     </row>
     <row r="5" spans="1:7" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
@@ -1347,7 +1347,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>8</v>
@@ -1370,13 +1370,13 @@
         <v>37</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>35</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -1387,7 +1387,7 @@
         <v>38</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>36</v>
@@ -1396,7 +1396,7 @@
         <v>3500000</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -1407,13 +1407,13 @@
         <v>39</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>35</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -1424,13 +1424,13 @@
         <v>12</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>35</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -1441,7 +1441,7 @@
         <v>40</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>41</v>
@@ -1458,7 +1458,7 @@
         <v>43</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>41</v>
@@ -1472,10 +1472,10 @@
         <v>46</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>36</v>
@@ -1492,16 +1492,16 @@
         <v>48</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>41</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -1509,16 +1509,16 @@
         <v>49</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>41</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -1526,16 +1526,16 @@
         <v>50</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>41</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -1543,16 +1543,16 @@
         <v>51</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>35</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -1560,10 +1560,10 @@
         <v>52</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D17" s="17" t="s">
         <v>35</v>
@@ -1574,16 +1574,16 @@
         <v>53</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D18" s="17" t="s">
         <v>35</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -1591,16 +1591,16 @@
         <v>54</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D19" s="17" t="s">
         <v>35</v>
       </c>
       <c r="E19" s="40" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -1608,10 +1608,10 @@
         <v>56</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D20" s="17" t="s">
         <v>36</v>
@@ -1625,10 +1625,10 @@
         <v>55</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>36</v>
@@ -1642,10 +1642,10 @@
         <v>57</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D22" s="17" t="s">
         <v>36</v>
@@ -1656,98 +1656,98 @@
     </row>
     <row r="23" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
-        <v>58</v>
+        <v>158</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>112</v>
+        <v>160</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D23" s="17" t="s">
         <v>41</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>76</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D24" s="17" t="s">
         <v>41</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D25" s="40" t="s">
         <v>41</v>
       </c>
       <c r="E25" s="40" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D26" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="E26" s="61" t="s">
-        <v>154</v>
+      <c r="E26" s="56" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D27" s="17" t="s">
         <v>35</v>
       </c>
       <c r="E27" s="40" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D28" s="17" t="s">
         <v>35</v>
@@ -1755,64 +1755,64 @@
     </row>
     <row r="29" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D29" s="17" t="s">
         <v>41</v>
       </c>
       <c r="E29" s="40" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D30" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="E30" s="61" t="s">
-        <v>156</v>
+      <c r="E30" s="56" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D31" s="17" t="s">
         <v>35</v>
       </c>
       <c r="E31" s="40" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D32" s="17" t="s">
         <v>36</v>
@@ -1823,64 +1823,64 @@
     </row>
     <row r="33" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D33" s="17" t="s">
         <v>41</v>
       </c>
       <c r="E33" s="40" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D34" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="E34" s="61" t="s">
-        <v>156</v>
+      <c r="E34" s="56" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D35" s="17" t="s">
         <v>35</v>
       </c>
       <c r="E35" s="40" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D36" s="17" t="s">
         <v>36</v>
@@ -1891,47 +1891,47 @@
     </row>
     <row r="37" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D37" s="40" t="s">
         <v>35</v>
       </c>
       <c r="E37" s="40" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D38" s="17" t="s">
         <v>35</v>
       </c>
       <c r="E38" s="40" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="C39" s="19" t="s">
         <v>95</v>
-      </c>
-      <c r="B39" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="C39" s="19" t="s">
-        <v>97</v>
       </c>
       <c r="D39" s="17" t="s">
         <v>36</v>
@@ -1942,13 +1942,13 @@
     </row>
     <row r="40" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D40" s="17" t="s">
         <v>36</v>
@@ -1959,13 +1959,13 @@
     </row>
     <row r="41" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B41" s="19" t="s">
         <v>1</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D41" s="17" t="s">
         <v>36</v>
@@ -1976,13 +1976,13 @@
     </row>
     <row r="42" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D42" s="17" t="s">
         <v>36</v>
@@ -1993,101 +1993,101 @@
     </row>
     <row r="43" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="15" t="s">
-        <v>77</v>
+        <v>157</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>129</v>
+        <v>160</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D43" s="17" t="s">
         <v>41</v>
       </c>
       <c r="E43" s="17" t="s">
-        <v>76</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C44" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D44" s="17" t="s">
         <v>41</v>
       </c>
       <c r="E44" s="17" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F44" s="17" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C45" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D45" s="17" t="s">
         <v>41</v>
       </c>
       <c r="E45" s="17" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C46" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D46" s="17" t="s">
         <v>41</v>
       </c>
       <c r="E46" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C47" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D47" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="E47" s="61" t="s">
-        <v>160</v>
+      <c r="E47" s="56" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C48" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D48" s="17" t="s">
         <v>35</v>
@@ -2098,41 +2098,41 @@
     </row>
     <row r="49" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C49" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C50" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D50" s="17" t="s">
         <v>41</v>
       </c>
       <c r="E50" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C51" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D51" s="17" t="s">
         <v>36</v>
@@ -2143,13 +2143,13 @@
     </row>
     <row r="52" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C52" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D52" s="17" t="s">
         <v>35</v>
@@ -2157,13 +2157,13 @@
     </row>
     <row r="53" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B53" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="C53" s="21" t="s">
         <v>92</v>
-      </c>
-      <c r="B53" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="C53" s="21" t="s">
-        <v>94</v>
       </c>
       <c r="D53" s="17" t="s">
         <v>35</v>
@@ -2171,13 +2171,13 @@
     </row>
     <row r="54" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C54" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D54" s="22" t="s">
         <v>36</v>
@@ -2195,14 +2195,14 @@
       <c r="C56" s="22"/>
     </row>
     <row r="57" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="44" t="s">
+      <c r="A57" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="B57" s="44"/>
-      <c r="C57" s="44"/>
-      <c r="D57" s="44"/>
-      <c r="E57" s="44"/>
-      <c r="F57" s="44"/>
+      <c r="B57" s="60"/>
+      <c r="C57" s="60"/>
+      <c r="D57" s="60"/>
+      <c r="E57" s="60"/>
+      <c r="F57" s="60"/>
     </row>
     <row r="58" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="9" t="s">
@@ -2212,7 +2212,7 @@
         <v>7</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D58" s="10" t="s">
         <v>8</v>
@@ -2236,7 +2236,7 @@
         <v>35</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2298,7 +2298,7 @@
         <v>26</v>
       </c>
       <c r="C63" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D63" s="17" t="s">
         <v>36</v>
@@ -2315,7 +2315,7 @@
         <v>27</v>
       </c>
       <c r="C64" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D64" s="17" t="s">
         <v>36</v>
@@ -2332,7 +2332,7 @@
         <v>20</v>
       </c>
       <c r="C65" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D65" s="17" t="s">
         <v>36</v>
@@ -2349,7 +2349,7 @@
         <v>28</v>
       </c>
       <c r="C66" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D66" s="17" t="s">
         <v>36</v>
@@ -2367,7 +2367,7 @@
         <v>29</v>
       </c>
       <c r="C67" s="27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D67" s="17" t="s">
         <v>36</v>
@@ -2384,7 +2384,7 @@
         <v>30</v>
       </c>
       <c r="C68" s="27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D68" s="17" t="s">
         <v>36</v>
@@ -2394,7 +2394,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="N0BtLGdWGAo56rAxBtdT0fUM8P0Sab7ZHYtlhuU3zw/NZ1EVMspFQF91bV/sBhX8fvMhzYmdxWikmYqSVc6Mlg==" saltValue="X7C9JnUdgrH+3aaOLEOf1g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="bWEfqtjWj6tSM1jFFVyVSyqhamczh+a2JbqA80RKae76D2L71RfXqxd575iwYxrIdshIgoOpFbiBaHluPjF1Mg==" saltValue="t8QZEo9VqzZ8PgQ4Ibz0iQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="5">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
@@ -2411,23 +2411,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ECE994F-BB82-2E4E-84AB-792F6F7C8F43}">
   <dimension ref="A1:AW1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="AL2" sqref="AL2:AL1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.83203125" defaultRowHeight="26" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="24.83203125" style="54"/>
-    <col min="6" max="6" width="24.83203125" style="55"/>
-    <col min="7" max="14" width="24.83203125" style="56"/>
-    <col min="15" max="16" width="24.83203125" style="57"/>
-    <col min="17" max="18" width="24.83203125" style="56"/>
-    <col min="19" max="26" width="24.83203125" style="58"/>
-    <col min="27" max="27" width="24.83203125" style="59"/>
-    <col min="28" max="38" width="24.83203125" style="58"/>
-    <col min="39" max="47" width="24.83203125" style="52"/>
-    <col min="48" max="49" width="24.83203125" style="60"/>
-    <col min="50" max="16384" width="24.83203125" style="49"/>
+    <col min="1" max="5" width="24.83203125" style="49"/>
+    <col min="6" max="6" width="24.83203125" style="50"/>
+    <col min="7" max="14" width="24.83203125" style="51"/>
+    <col min="15" max="16" width="24.83203125" style="52"/>
+    <col min="17" max="18" width="24.83203125" style="51"/>
+    <col min="19" max="26" width="24.83203125" style="53"/>
+    <col min="27" max="27" width="24.83203125" style="54"/>
+    <col min="28" max="38" width="24.83203125" style="53"/>
+    <col min="39" max="47" width="24.83203125" style="47"/>
+    <col min="48" max="49" width="24.83203125" style="55"/>
+    <col min="50" max="16384" width="24.83203125" style="44"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:49" s="6" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -2483,104 +2483,104 @@
         <v>57</v>
       </c>
       <c r="R1" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="S1" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="S1" s="31" t="s">
+      <c r="T1" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="T1" s="31" t="s">
+      <c r="U1" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="U1" s="31" t="s">
+      <c r="V1" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="V1" s="31" t="s">
+      <c r="W1" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="W1" s="31" t="s">
+      <c r="X1" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="X1" s="31" t="s">
+      <c r="Y1" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="Y1" s="31" t="s">
+      <c r="Z1" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="Z1" s="31" t="s">
+      <c r="AA1" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="AA1" s="31" t="s">
+      <c r="AB1" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="AB1" s="31" t="s">
+      <c r="AC1" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="AC1" s="31" t="s">
+      <c r="AD1" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="AD1" s="31" t="s">
+      <c r="AE1" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="AE1" s="31" t="s">
-        <v>71</v>
-      </c>
       <c r="AF1" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="AG1" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="AH1" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="AI1" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="AJ1" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="AG1" s="31" t="s">
+      <c r="AK1" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="AH1" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="AI1" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="AJ1" s="31" t="s">
+      <c r="AL1" s="31" t="s">
+        <v>157</v>
+      </c>
+      <c r="AM1" s="38" t="s">
+        <v>81</v>
+      </c>
+      <c r="AN1" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="AK1" s="37" t="s">
-        <v>81</v>
-      </c>
-      <c r="AL1" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="AM1" s="38" t="s">
-        <v>83</v>
-      </c>
-      <c r="AN1" s="39" t="s">
+      <c r="AO1" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="AO1" s="38" t="s">
+      <c r="AP1" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="AQ1" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="AP1" s="32" t="s">
+      <c r="AR1" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="AS1" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="AQ1" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="AR1" s="32" t="s">
+      <c r="AT1" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="AS1" s="32" t="s">
+      <c r="AU1" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="AT1" s="32" t="s">
+      <c r="AV1" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="AU1" s="32" t="s">
+      <c r="AW1" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="AV1" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="AW1" s="39" t="s">
-        <v>93</v>
-      </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="dzcmAfGou4weLrVvywGvnQuR58ds7aGJNoG2Slxtp8/KVs+eOWKsJP/3yNsXFmAFlaVNFnKZgJxX7QOp8aVMJA==" saltValue="TS0L2MsAB7gnj79lYkTz/g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="nJnIa2kb7Lm7+KXR7fG+b+MyzezHJBdfRDjnwDgTiQdjRIRynCq17jslkbfdwvsMW0iwdLAYh+cULn/eH4paNw==" saltValue="SA0c9XXSOjwQ4fQnoMXBJA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="45">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="&lt;lab-name&gt;_Illumina_D5_&lt;sequencing-date&gt;_&lt;no.&gt;_R1/R2.fastq.gz_x000d__x000a__x000d__x000a_e.g FDU_Illumina_D5_20200808_001_R1.fastq.gz" sqref="B2:B1048576" xr:uid="{EE4EBFB8-3AF4-9545-A3BA-CB54EA5CFE04}"/>
@@ -2619,8 +2619,8 @@
       <formula1>19000000</formula1>
       <formula2>21000000</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Is automation?" prompt="e.g. TRUE" sqref="R2:R1048576" xr:uid="{75FDDACF-6B09-C24D-98C5-AA2BA50E61AE}">
-      <formula1>"TRUE,FALSE"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Manual or automated enrichment" prompt="e.g. Manual" sqref="R2:R1048576" xr:uid="{75FDDACF-6B09-C24D-98C5-AA2BA50E61AE}">
+      <formula1>"Manual,Automated"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Is strand specific?" prompt="e.g. TRUE" sqref="S2:S1048576" xr:uid="{56529B1E-7C9A-D842-9445-6B685BFFA2C5}">
       <formula1>"TRUE,FALSE"</formula1>
@@ -2660,8 +2660,8 @@
       <formula1>19000000</formula1>
       <formula2>21000000</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2:AL1048576" xr:uid="{B4EB32C1-D74B-8E49-B11C-C4C5C43ADEBD}">
-      <formula1>"TRUE,FALSE"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Manual or automated library prep" prompt="e.g. Manual" sqref="AL2:AL1048576" xr:uid="{B4EB32C1-D74B-8E49-B11C-C4C5C43ADEBD}">
+      <formula1>"Manual,Automated"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Manufacturer for sequencer" prompt="e.g. Illumina" sqref="AM2:AM1048576" xr:uid="{D9C6F851-7E62-1B48-B1A2-9EC369BEA4B9}">
       <formula1>"Illumina,MGI"</formula1>
@@ -2699,11 +2699,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="49"/>
-    <col min="2" max="4" width="20.6640625" style="52"/>
-    <col min="5" max="8" width="20.6640625" style="53"/>
-    <col min="9" max="10" width="20.6640625" style="48"/>
-    <col min="11" max="16384" width="20.6640625" style="47"/>
+    <col min="1" max="1" width="20.6640625" style="44"/>
+    <col min="2" max="4" width="20.6640625" style="47"/>
+    <col min="5" max="8" width="20.6640625" style="48"/>
+    <col min="9" max="10" width="20.6640625" style="43"/>
+    <col min="11" max="16384" width="20.6640625" style="42"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2739,15 +2739,15 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="/c/p3vurwIDKYkaMV70rveWOgGayM+u2lEe9LX1UjTBPjUenRCBWQzVLynBoreHbIMczw3qiCjZ8pJ0vOVVwNg==" saltValue="E8OgBx0mVtKE+UgmG47uCw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>

</xml_diff>